<commit_message>
uloha_03: Dokončení úkolů 3 a 4.
</commit_message>
<xml_diff>
--- a/uloha_03/data_03/data_03.xlsx
+++ b/uloha_03/data_03/data_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V-A charakteristika" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t xml:space="preserve">t [\mu s]</t>
   </si>
@@ -32,10 +32,7 @@
     <t xml:space="preserve">U_mer [V]</t>
   </si>
   <si>
-    <t xml:space="preserve">U_RI [mV]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U_F [mV]</t>
+    <t xml:space="preserve">U_F [V]</t>
   </si>
 </sst>
 </file>
@@ -628,11 +625,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13982388"/>
-        <c:axId val="15252196"/>
+        <c:axId val="76872400"/>
+        <c:axId val="31505339"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13982388"/>
+        <c:axId val="76872400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,12 +661,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15252196"/>
+        <c:crossAx val="31505339"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="15252196"/>
+        <c:axId val="31505339"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +707,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13982388"/>
+        <c:crossAx val="76872400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -910,7 +907,7 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -1524,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1535,10 +1532,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>